<commit_message>
Add home feature added and method name change
</commit_message>
<xml_diff>
--- a/TestData/AddBuildingdata.xlsx
+++ b/TestData/AddBuildingdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS238\PycharmProjects\Abra_Platform_Automation_Testing_Using_Python\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F9B756-5F37-409F-8E30-C45127B0CAA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF753428-802B-454B-BBFE-F8F1DC53A39D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{C135F285-4FB4-442E-94FE-9031FDE1FD1B}"/>
   </bookViews>
@@ -91,10 +91,10 @@
     <t>Type Three</t>
   </si>
   <si>
-    <t>Testing add building(Anan)</t>
-  </si>
-  <si>
-    <t>C://Users\BS238\PycharmProjects\Abra_Platform_Automation_Testing_Using_Python\TestData\image1.jpg</t>
+    <t>Add New Building TWO (3/9/2022(Anan))</t>
+  </si>
+  <si>
+    <t>C://Users\BS238\PycharmProjects\Abra_Platform_Automation_Testing_Using_Python\TestData\BS23.png</t>
   </si>
 </sst>
 </file>
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,7 +147,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,24 +471,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C5757A-DBE1-4D97-8EBA-75B6C14C8024}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="44" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22" style="4" customWidth="1"/>
+    <col min="4" max="5" width="20.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="44" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -527,43 +533,43 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1207</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="3">
         <v>2022</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="3">
         <v>2</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -578,7 +584,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>